<commit_message>
Updated Image & documents
</commit_message>
<xml_diff>
--- a/Resources/Jmeter_load_testing.xlsx
+++ b/Resources/Jmeter_load_testing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devnet\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Road-to-SDET\jmeter-project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66610912-8039-47F6-8D84-988D6844F26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9753E138-28B2-45EE-AC47-0B237A096E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{55C8AA13-912A-4331-9BD1-061BA310AD21}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Actual TPS</t>
   </si>
@@ -74,17 +74,23 @@
     <t>Test 3</t>
   </si>
   <si>
-    <t>Throughput</t>
-  </si>
-  <si>
-    <t>Server URL: demoqa.com</t>
+    <t>Load Test Strategy</t>
+  </si>
+  <si>
+    <t>Server URL: demoqa.com/BookStore/v1/Books</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>The load test has been successful as opposed to the expected load</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +133,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
@@ -159,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,12 +179,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -208,11 +213,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,31 +274,55 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D663C0-3622-4D3E-8BA0-2F4F4CA57472}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,31 +653,33 @@
     <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -627,15 +695,15 @@
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="G3" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
@@ -650,11 +718,13 @@
       <c r="E4" s="2">
         <v>10000</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
@@ -666,11 +736,11 @@
         <f>E4/D4</f>
         <v>2.7777777777777777</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5"/>
@@ -684,15 +754,13 @@
         <f>E5*D6</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="23">
         <v>0</v>
       </c>
-      <c r="G6" s="5">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5"/>
@@ -706,15 +774,13 @@
         <f>E5*D7</f>
         <v>833.33333333333326</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="23">
         <v>0</v>
       </c>
-      <c r="G7" s="5">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
@@ -728,15 +794,13 @@
         <f>E5*D8</f>
         <v>1666.6666666666665</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="23">
         <v>0</v>
       </c>
-      <c r="G8" s="5">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="5"/>
@@ -750,35 +814,35 @@
         <f>D9*E5</f>
         <v>2500</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="23">
         <v>0</v>
       </c>
-      <c r="G9" s="5">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9">
-        <f>AVERAGE(G6:G9)</f>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G2"/>
+  <mergeCells count="3">
+    <mergeCell ref="G4:G9"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>